<commit_message>
fixed 'more than ne try per node' problem
</commit_message>
<xml_diff>
--- a/8/evaluation.xlsx
+++ b/8/evaluation.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Chart1" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Chart1" sheetId="2" r:id="rId2"/>
+    <sheet name="Chart1 (2)" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="2">
   <si>
     <t>deg</t>
   </si>
@@ -1444,7 +1445,1453 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-AT"/>
+              <a:t>Knotengradverteilung für preferential attachment</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-AT" baseline="0"/>
+              <a:t> graph (n=10000)</a:t>
+            </a:r>
+            <a:endParaRPr lang="de-AT"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Lauf 1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$5:$L$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>167</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$M$5:$M$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+                <c:pt idx="0">
+                  <c:v>6746</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1580</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>636</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>366</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>206</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-4FD0-4C8A-B04E-3A0BEBD55F21}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Lauf 2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$O$5:$O$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="47"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>57</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$5:$P$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="47"/>
+                <c:pt idx="0">
+                  <c:v>6633</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1679</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>343</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-4FD0-4C8A-B04E-3A0BEBD55F21}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Lauf 3</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$R$5:$R$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="44"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>57</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$S$5:$S$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="44"/>
+                <c:pt idx="0">
+                  <c:v>6655</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1674</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>670</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>334</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>188</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-4FD0-4C8A-B04E-3A0BEBD55F21}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="283225360"/>
+        <c:axId val="283223720"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="283225360"/>
+        <c:scaling>
+          <c:logBase val="2"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-AT"/>
+                  <a:t>Knotengrad x</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="283223720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="283223720"/>
+        <c:scaling>
+          <c:logBase val="2"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-AT"/>
+                  <a:t>Anzahl</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-AT" baseline="0"/>
+                  <a:t> Knoten mit Grad x</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-AT"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="283225360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2000,7 +3447,534 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
@@ -2022,6 +3996,39 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DFD29D4-C46E-46FE-AFB5-C7B0A431ACB6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9304587" cy="6077107"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF875D20-A55B-49E6-AF05-75494E8E1133}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2307,15 +4314,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:J51"/>
+  <dimension ref="C3:S51"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5:S49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C3">
         <v>1</v>
       </c>
@@ -2325,8 +4332,17 @@
       <c r="I3">
         <v>3</v>
       </c>
+      <c r="L3">
+        <v>4</v>
+      </c>
+      <c r="O3">
+        <v>5</v>
+      </c>
+      <c r="R3">
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>0</v>
       </c>
@@ -2345,8 +4361,26 @@
       <c r="J4" t="s">
         <v>1</v>
       </c>
+      <c r="L4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" t="s">
+        <v>0</v>
+      </c>
+      <c r="P4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R4" t="s">
+        <v>0</v>
+      </c>
+      <c r="S4" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>1</v>
       </c>
@@ -2365,8 +4399,26 @@
       <c r="J5">
         <v>6697</v>
       </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>6746</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>6633</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>6655</v>
+      </c>
     </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>2</v>
       </c>
@@ -2385,8 +4437,26 @@
       <c r="J6">
         <v>1645</v>
       </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <v>1580</v>
+      </c>
+      <c r="O6">
+        <v>2</v>
+      </c>
+      <c r="P6">
+        <v>1679</v>
+      </c>
+      <c r="R6">
+        <v>2</v>
+      </c>
+      <c r="S6">
+        <v>1674</v>
+      </c>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>3</v>
       </c>
@@ -2405,8 +4475,26 @@
       <c r="J7">
         <v>652</v>
       </c>
+      <c r="L7">
+        <v>3</v>
+      </c>
+      <c r="M7">
+        <v>636</v>
+      </c>
+      <c r="O7">
+        <v>3</v>
+      </c>
+      <c r="P7">
+        <v>680</v>
+      </c>
+      <c r="R7">
+        <v>3</v>
+      </c>
+      <c r="S7">
+        <v>670</v>
+      </c>
     </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>4</v>
       </c>
@@ -2425,8 +4513,26 @@
       <c r="J8">
         <v>360</v>
       </c>
+      <c r="L8">
+        <v>4</v>
+      </c>
+      <c r="M8">
+        <v>366</v>
+      </c>
+      <c r="O8">
+        <v>4</v>
+      </c>
+      <c r="P8">
+        <v>343</v>
+      </c>
+      <c r="R8">
+        <v>4</v>
+      </c>
+      <c r="S8">
+        <v>334</v>
+      </c>
     </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>5</v>
       </c>
@@ -2445,8 +4551,26 @@
       <c r="J9">
         <v>181</v>
       </c>
+      <c r="L9">
+        <v>5</v>
+      </c>
+      <c r="M9">
+        <v>206</v>
+      </c>
+      <c r="O9">
+        <v>5</v>
+      </c>
+      <c r="P9">
+        <v>190</v>
+      </c>
+      <c r="R9">
+        <v>5</v>
+      </c>
+      <c r="S9">
+        <v>188</v>
+      </c>
     </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>6</v>
       </c>
@@ -2465,8 +4589,26 @@
       <c r="J10">
         <v>112</v>
       </c>
+      <c r="L10">
+        <v>6</v>
+      </c>
+      <c r="M10">
+        <v>114</v>
+      </c>
+      <c r="O10">
+        <v>6</v>
+      </c>
+      <c r="P10">
+        <v>132</v>
+      </c>
+      <c r="R10">
+        <v>70</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>7</v>
       </c>
@@ -2485,8 +4627,26 @@
       <c r="J11">
         <v>85</v>
       </c>
+      <c r="L11">
+        <v>7</v>
+      </c>
+      <c r="M11">
+        <v>82</v>
+      </c>
+      <c r="O11">
+        <v>7</v>
+      </c>
+      <c r="P11">
+        <v>73</v>
+      </c>
+      <c r="R11">
+        <v>6</v>
+      </c>
+      <c r="S11">
+        <v>125</v>
+      </c>
     </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>8</v>
       </c>
@@ -2505,8 +4665,26 @@
       <c r="J12">
         <v>46</v>
       </c>
+      <c r="L12">
+        <v>8</v>
+      </c>
+      <c r="M12">
+        <v>49</v>
+      </c>
+      <c r="O12">
+        <v>71</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <v>7</v>
+      </c>
+      <c r="S12">
+        <v>73</v>
+      </c>
     </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>9</v>
       </c>
@@ -2525,8 +4703,26 @@
       <c r="J13">
         <v>44</v>
       </c>
+      <c r="L13">
+        <v>9</v>
+      </c>
+      <c r="M13">
+        <v>41</v>
+      </c>
+      <c r="O13">
+        <v>72</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="R13">
+        <v>8</v>
+      </c>
+      <c r="S13">
+        <v>58</v>
+      </c>
     </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>10</v>
       </c>
@@ -2545,8 +4741,26 @@
       <c r="J14">
         <v>35</v>
       </c>
+      <c r="L14">
+        <v>10</v>
+      </c>
+      <c r="M14">
+        <v>27</v>
+      </c>
+      <c r="O14">
+        <v>8</v>
+      </c>
+      <c r="P14">
+        <v>50</v>
+      </c>
+      <c r="R14">
+        <v>72</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>11</v>
       </c>
@@ -2565,8 +4779,26 @@
       <c r="J15">
         <v>26</v>
       </c>
+      <c r="L15">
+        <v>11</v>
+      </c>
+      <c r="M15">
+        <v>19</v>
+      </c>
+      <c r="O15">
+        <v>9</v>
+      </c>
+      <c r="P15">
+        <v>32</v>
+      </c>
+      <c r="R15">
+        <v>9</v>
+      </c>
+      <c r="S15">
+        <v>35</v>
+      </c>
     </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>12</v>
       </c>
@@ -2585,8 +4817,26 @@
       <c r="J16">
         <v>20</v>
       </c>
+      <c r="L16">
+        <v>12</v>
+      </c>
+      <c r="M16">
+        <v>22</v>
+      </c>
+      <c r="O16">
+        <v>10</v>
+      </c>
+      <c r="P16">
+        <v>42</v>
+      </c>
+      <c r="R16">
+        <v>10</v>
+      </c>
+      <c r="S16">
+        <v>28</v>
+      </c>
     </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>13</v>
       </c>
@@ -2605,8 +4855,26 @@
       <c r="J17">
         <v>9</v>
       </c>
+      <c r="L17">
+        <v>13</v>
+      </c>
+      <c r="M17">
+        <v>13</v>
+      </c>
+      <c r="O17">
+        <v>11</v>
+      </c>
+      <c r="P17">
+        <v>21</v>
+      </c>
+      <c r="R17">
+        <v>11</v>
+      </c>
+      <c r="S17">
+        <v>30</v>
+      </c>
     </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C18">
         <v>14</v>
       </c>
@@ -2625,8 +4893,26 @@
       <c r="J18">
         <v>6</v>
       </c>
+      <c r="L18">
+        <v>14</v>
+      </c>
+      <c r="M18">
+        <v>18</v>
+      </c>
+      <c r="O18">
+        <v>12</v>
+      </c>
+      <c r="P18">
+        <v>14</v>
+      </c>
+      <c r="R18">
+        <v>12</v>
+      </c>
+      <c r="S18">
+        <v>23</v>
+      </c>
     </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>15</v>
       </c>
@@ -2645,8 +4931,26 @@
       <c r="J19">
         <v>12</v>
       </c>
+      <c r="L19">
+        <v>15</v>
+      </c>
+      <c r="M19">
+        <v>11</v>
+      </c>
+      <c r="O19">
+        <v>13</v>
+      </c>
+      <c r="P19">
+        <v>16</v>
+      </c>
+      <c r="R19">
+        <v>13</v>
+      </c>
+      <c r="S19">
+        <v>11</v>
+      </c>
     </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>16</v>
       </c>
@@ -2665,8 +4969,26 @@
       <c r="J20">
         <v>6</v>
       </c>
+      <c r="L20">
+        <v>16</v>
+      </c>
+      <c r="M20">
+        <v>11</v>
+      </c>
+      <c r="O20">
+        <v>14</v>
+      </c>
+      <c r="P20">
+        <v>10</v>
+      </c>
+      <c r="R20">
+        <v>14</v>
+      </c>
+      <c r="S20">
+        <v>12</v>
+      </c>
     </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>17</v>
       </c>
@@ -2685,8 +5007,26 @@
       <c r="J21">
         <v>9</v>
       </c>
+      <c r="L21">
+        <v>17</v>
+      </c>
+      <c r="M21">
+        <v>6</v>
+      </c>
+      <c r="O21">
+        <v>15</v>
+      </c>
+      <c r="P21">
+        <v>8</v>
+      </c>
+      <c r="R21">
+        <v>15</v>
+      </c>
+      <c r="S21">
+        <v>6</v>
+      </c>
     </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>18</v>
       </c>
@@ -2705,8 +5045,26 @@
       <c r="J22">
         <v>8</v>
       </c>
+      <c r="L22">
+        <v>18</v>
+      </c>
+      <c r="M22">
+        <v>2</v>
+      </c>
+      <c r="O22">
+        <v>80</v>
+      </c>
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="R22">
+        <v>16</v>
+      </c>
+      <c r="S22">
+        <v>13</v>
+      </c>
     </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>19</v>
       </c>
@@ -2725,8 +5083,26 @@
       <c r="J23">
         <v>1</v>
       </c>
+      <c r="L23">
+        <v>19</v>
+      </c>
+      <c r="M23">
+        <v>11</v>
+      </c>
+      <c r="O23">
+        <v>16</v>
+      </c>
+      <c r="P23">
+        <v>11</v>
+      </c>
+      <c r="R23">
+        <v>17</v>
+      </c>
+      <c r="S23">
+        <v>9</v>
+      </c>
     </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C24">
         <v>20</v>
       </c>
@@ -2745,8 +5121,26 @@
       <c r="J24">
         <v>5</v>
       </c>
+      <c r="L24">
+        <v>20</v>
+      </c>
+      <c r="M24">
+        <v>2</v>
+      </c>
+      <c r="O24">
+        <v>17</v>
+      </c>
+      <c r="P24">
+        <v>8</v>
+      </c>
+      <c r="R24">
+        <v>18</v>
+      </c>
+      <c r="S24">
+        <v>5</v>
+      </c>
     </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C25">
         <v>21</v>
       </c>
@@ -2765,8 +5159,26 @@
       <c r="J25">
         <v>1</v>
       </c>
+      <c r="L25">
+        <v>22</v>
+      </c>
+      <c r="M25">
+        <v>3</v>
+      </c>
+      <c r="O25">
+        <v>18</v>
+      </c>
+      <c r="P25">
+        <v>3</v>
+      </c>
+      <c r="R25">
+        <v>19</v>
+      </c>
+      <c r="S25">
+        <v>2</v>
+      </c>
     </row>
-    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>22</v>
       </c>
@@ -2785,8 +5197,26 @@
       <c r="J26">
         <v>2</v>
       </c>
+      <c r="L26">
+        <v>23</v>
+      </c>
+      <c r="M26">
+        <v>2</v>
+      </c>
+      <c r="O26">
+        <v>19</v>
+      </c>
+      <c r="P26">
+        <v>1</v>
+      </c>
+      <c r="R26">
+        <v>20</v>
+      </c>
+      <c r="S26">
+        <v>4</v>
+      </c>
     </row>
-    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>23</v>
       </c>
@@ -2805,8 +5235,26 @@
       <c r="J27">
         <v>6</v>
       </c>
+      <c r="L27">
+        <v>24</v>
+      </c>
+      <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>20</v>
+      </c>
+      <c r="P27">
+        <v>5</v>
+      </c>
+      <c r="R27">
+        <v>21</v>
+      </c>
+      <c r="S27">
+        <v>5</v>
+      </c>
     </row>
-    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C28">
         <v>24</v>
       </c>
@@ -2825,8 +5273,26 @@
       <c r="J28">
         <v>2</v>
       </c>
+      <c r="L28">
+        <v>25</v>
+      </c>
+      <c r="M28">
+        <v>4</v>
+      </c>
+      <c r="O28">
+        <v>21</v>
+      </c>
+      <c r="P28">
+        <v>4</v>
+      </c>
+      <c r="R28">
+        <v>22</v>
+      </c>
+      <c r="S28">
+        <v>7</v>
+      </c>
     </row>
-    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C29">
         <v>26</v>
       </c>
@@ -2845,8 +5311,26 @@
       <c r="J29">
         <v>2</v>
       </c>
+      <c r="L29">
+        <v>27</v>
+      </c>
+      <c r="M29">
+        <v>2</v>
+      </c>
+      <c r="O29">
+        <v>22</v>
+      </c>
+      <c r="P29">
+        <v>4</v>
+      </c>
+      <c r="R29">
+        <v>23</v>
+      </c>
+      <c r="S29">
+        <v>1</v>
+      </c>
     </row>
-    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C30">
         <v>27</v>
       </c>
@@ -2865,8 +5349,26 @@
       <c r="J30">
         <v>1</v>
       </c>
+      <c r="L30">
+        <v>28</v>
+      </c>
+      <c r="M30">
+        <v>3</v>
+      </c>
+      <c r="O30">
+        <v>23</v>
+      </c>
+      <c r="P30">
+        <v>3</v>
+      </c>
+      <c r="R30">
+        <v>24</v>
+      </c>
+      <c r="S30">
+        <v>2</v>
+      </c>
     </row>
-    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C31">
         <v>30</v>
       </c>
@@ -2885,8 +5387,26 @@
       <c r="J31">
         <v>1</v>
       </c>
+      <c r="L31">
+        <v>29</v>
+      </c>
+      <c r="M31">
+        <v>1</v>
+      </c>
+      <c r="O31">
+        <v>24</v>
+      </c>
+      <c r="P31">
+        <v>1</v>
+      </c>
+      <c r="R31">
+        <v>25</v>
+      </c>
+      <c r="S31">
+        <v>1</v>
+      </c>
     </row>
-    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C32">
         <v>31</v>
       </c>
@@ -2905,8 +5425,26 @@
       <c r="J32">
         <v>2</v>
       </c>
+      <c r="L32">
+        <v>31</v>
+      </c>
+      <c r="M32">
+        <v>1</v>
+      </c>
+      <c r="O32">
+        <v>25</v>
+      </c>
+      <c r="P32">
+        <v>2</v>
+      </c>
+      <c r="R32">
+        <v>26</v>
+      </c>
+      <c r="S32">
+        <v>3</v>
+      </c>
     </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C33">
         <v>32</v>
       </c>
@@ -2925,8 +5463,26 @@
       <c r="J33">
         <v>4</v>
       </c>
+      <c r="L33">
+        <v>32</v>
+      </c>
+      <c r="M33">
+        <v>1</v>
+      </c>
+      <c r="O33">
+        <v>26</v>
+      </c>
+      <c r="P33">
+        <v>3</v>
+      </c>
+      <c r="R33">
+        <v>27</v>
+      </c>
+      <c r="S33">
+        <v>3</v>
+      </c>
     </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C34">
         <v>33</v>
       </c>
@@ -2945,8 +5501,26 @@
       <c r="J34">
         <v>2</v>
       </c>
+      <c r="L34">
+        <v>33</v>
+      </c>
+      <c r="M34">
+        <v>1</v>
+      </c>
+      <c r="O34">
+        <v>27</v>
+      </c>
+      <c r="P34">
+        <v>3</v>
+      </c>
+      <c r="R34">
+        <v>28</v>
+      </c>
+      <c r="S34">
+        <v>1</v>
+      </c>
     </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C35">
         <v>35</v>
       </c>
@@ -2965,8 +5539,26 @@
       <c r="J35">
         <v>1</v>
       </c>
+      <c r="L35">
+        <v>34</v>
+      </c>
+      <c r="M35">
+        <v>2</v>
+      </c>
+      <c r="O35">
+        <v>28</v>
+      </c>
+      <c r="P35">
+        <v>2</v>
+      </c>
+      <c r="R35">
+        <v>30</v>
+      </c>
+      <c r="S35">
+        <v>1</v>
+      </c>
     </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C36">
         <v>36</v>
       </c>
@@ -2985,8 +5577,26 @@
       <c r="J36">
         <v>1</v>
       </c>
+      <c r="L36">
+        <v>39</v>
+      </c>
+      <c r="M36">
+        <v>2</v>
+      </c>
+      <c r="O36">
+        <v>29</v>
+      </c>
+      <c r="P36">
+        <v>2</v>
+      </c>
+      <c r="R36">
+        <v>31</v>
+      </c>
+      <c r="S36">
+        <v>2</v>
+      </c>
     </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C37">
         <v>38</v>
       </c>
@@ -3005,8 +5615,26 @@
       <c r="J37">
         <v>1</v>
       </c>
+      <c r="L37">
+        <v>41</v>
+      </c>
+      <c r="M37">
+        <v>3</v>
+      </c>
+      <c r="O37">
+        <v>30</v>
+      </c>
+      <c r="P37">
+        <v>4</v>
+      </c>
+      <c r="R37">
+        <v>32</v>
+      </c>
+      <c r="S37">
+        <v>1</v>
+      </c>
     </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C38">
         <v>40</v>
       </c>
@@ -3025,8 +5653,26 @@
       <c r="J38">
         <v>2</v>
       </c>
+      <c r="L38">
+        <v>45</v>
+      </c>
+      <c r="M38">
+        <v>1</v>
+      </c>
+      <c r="O38">
+        <v>33</v>
+      </c>
+      <c r="P38">
+        <v>3</v>
+      </c>
+      <c r="R38">
+        <v>34</v>
+      </c>
+      <c r="S38">
+        <v>1</v>
+      </c>
     </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C39">
         <v>43</v>
       </c>
@@ -3045,8 +5691,26 @@
       <c r="J39">
         <v>1</v>
       </c>
+      <c r="L39">
+        <v>48</v>
+      </c>
+      <c r="M39">
+        <v>1</v>
+      </c>
+      <c r="O39">
+        <v>34</v>
+      </c>
+      <c r="P39">
+        <v>1</v>
+      </c>
+      <c r="R39">
+        <v>99</v>
+      </c>
+      <c r="S39">
+        <v>1</v>
+      </c>
     </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C40">
         <v>45</v>
       </c>
@@ -3065,8 +5729,26 @@
       <c r="J40">
         <v>1</v>
       </c>
+      <c r="L40">
+        <v>49</v>
+      </c>
+      <c r="M40">
+        <v>1</v>
+      </c>
+      <c r="O40">
+        <v>35</v>
+      </c>
+      <c r="P40">
+        <v>1</v>
+      </c>
+      <c r="R40">
+        <v>36</v>
+      </c>
+      <c r="S40">
+        <v>1</v>
+      </c>
     </row>
-    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C41">
         <v>46</v>
       </c>
@@ -3085,8 +5767,26 @@
       <c r="J41">
         <v>1</v>
       </c>
+      <c r="L41">
+        <v>60</v>
+      </c>
+      <c r="M41">
+        <v>1</v>
+      </c>
+      <c r="O41">
+        <v>38</v>
+      </c>
+      <c r="P41">
+        <v>1</v>
+      </c>
+      <c r="R41">
+        <v>38</v>
+      </c>
+      <c r="S41">
+        <v>1</v>
+      </c>
     </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C42">
         <v>47</v>
       </c>
@@ -3099,8 +5799,26 @@
       <c r="J42">
         <v>1</v>
       </c>
+      <c r="L42">
+        <v>67</v>
+      </c>
+      <c r="M42">
+        <v>1</v>
+      </c>
+      <c r="O42">
+        <v>232</v>
+      </c>
+      <c r="P42">
+        <v>1</v>
+      </c>
+      <c r="R42">
+        <v>40</v>
+      </c>
+      <c r="S42">
+        <v>2</v>
+      </c>
     </row>
-    <row r="43" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C43">
         <v>48</v>
       </c>
@@ -3117,8 +5835,26 @@
       <c r="J43">
         <v>1</v>
       </c>
+      <c r="L43">
+        <v>76</v>
+      </c>
+      <c r="M43">
+        <v>1</v>
+      </c>
+      <c r="O43">
+        <v>41</v>
+      </c>
+      <c r="P43">
+        <v>2</v>
+      </c>
+      <c r="R43">
+        <v>104</v>
+      </c>
+      <c r="S43">
+        <v>1</v>
+      </c>
     </row>
-    <row r="44" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C44">
         <v>49</v>
       </c>
@@ -3131,8 +5867,26 @@
       <c r="J44">
         <v>1</v>
       </c>
+      <c r="L44">
+        <v>79</v>
+      </c>
+      <c r="M44">
+        <v>1</v>
+      </c>
+      <c r="O44">
+        <v>42</v>
+      </c>
+      <c r="P44">
+        <v>1</v>
+      </c>
+      <c r="R44">
+        <v>41</v>
+      </c>
+      <c r="S44">
+        <v>4</v>
+      </c>
     </row>
-    <row r="45" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C45">
         <v>50</v>
       </c>
@@ -3145,8 +5899,26 @@
       <c r="J45">
         <v>1</v>
       </c>
+      <c r="L45">
+        <v>90</v>
+      </c>
+      <c r="M45">
+        <v>1</v>
+      </c>
+      <c r="O45">
+        <v>44</v>
+      </c>
+      <c r="P45">
+        <v>1</v>
+      </c>
+      <c r="R45">
+        <v>106</v>
+      </c>
+      <c r="S45">
+        <v>1</v>
+      </c>
     </row>
-    <row r="46" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C46">
         <v>70</v>
       </c>
@@ -3159,8 +5931,26 @@
       <c r="J46">
         <v>1</v>
       </c>
+      <c r="L46">
+        <v>96</v>
+      </c>
+      <c r="M46">
+        <v>1</v>
+      </c>
+      <c r="O46">
+        <v>45</v>
+      </c>
+      <c r="P46">
+        <v>1</v>
+      </c>
+      <c r="R46">
+        <v>48</v>
+      </c>
+      <c r="S46">
+        <v>1</v>
+      </c>
     </row>
-    <row r="47" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C47">
         <v>81</v>
       </c>
@@ -3173,8 +5963,26 @@
       <c r="J47">
         <v>1</v>
       </c>
+      <c r="L47">
+        <v>98</v>
+      </c>
+      <c r="M47">
+        <v>1</v>
+      </c>
+      <c r="O47">
+        <v>46</v>
+      </c>
+      <c r="P47">
+        <v>1</v>
+      </c>
+      <c r="R47">
+        <v>182</v>
+      </c>
+      <c r="S47">
+        <v>1</v>
+      </c>
     </row>
-    <row r="48" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C48">
         <v>176</v>
       </c>
@@ -3187,8 +5995,26 @@
       <c r="J48">
         <v>1</v>
       </c>
+      <c r="L48">
+        <v>136</v>
+      </c>
+      <c r="M48">
+        <v>1</v>
+      </c>
+      <c r="O48">
+        <v>48</v>
+      </c>
+      <c r="P48">
+        <v>1</v>
+      </c>
+      <c r="R48">
+        <v>57</v>
+      </c>
+      <c r="S48">
+        <v>2</v>
+      </c>
     </row>
-    <row r="49" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C49">
         <v>198</v>
       </c>
@@ -3201,16 +6027,34 @@
       <c r="J49">
         <v>1</v>
       </c>
+      <c r="L49">
+        <v>167</v>
+      </c>
+      <c r="M49">
+        <v>1</v>
+      </c>
+      <c r="O49">
+        <v>49</v>
+      </c>
+      <c r="P49">
+        <v>2</v>
+      </c>
     </row>
-    <row r="50" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:16" x14ac:dyDescent="0.25">
       <c r="I50">
         <v>159</v>
       </c>
       <c r="J50">
         <v>1</v>
       </c>
+      <c r="O50">
+        <v>51</v>
+      </c>
+      <c r="P50">
+        <v>1</v>
+      </c>
     </row>
-    <row r="51" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:16" x14ac:dyDescent="0.25">
       <c r="D51">
         <f>SUM(D5:D49)</f>
         <v>10000</v>
@@ -3221,10 +6065,16 @@
       <c r="J51">
         <v>1</v>
       </c>
+      <c r="O51">
+        <v>57</v>
+      </c>
+      <c r="P51">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="I5:J51">
-    <sortCondition ref="I5:I51"/>
+  <sortState ref="L5:M49">
+    <sortCondition ref="L5:L49"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>